<commit_message>
Fixing Dyck1_Counter_9_early_stopping to evaluate training set before training and stopping if no training is needed
</commit_message>
<xml_diff>
--- a/Dyck 1 Counter/Dyck1_Counter_9_early_stopping_Clipping_L1.xlsx
+++ b/Dyck 1 Counter/Dyck1_Counter_9_early_stopping_Clipping_L1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
   <si>
     <t>epochs</t>
   </si>
@@ -102,6 +102,9 @@
   <si>
     <t>[[ 1.  1.]
  [-1. -1.]]</t>
+  </si>
+  <si>
+    <t>No training occurred</t>
   </si>
 </sst>
 </file>
@@ -591,11 +594,11 @@
       <c r="T2" t="s">
         <v>21</v>
       </c>
-      <c r="U2">
-        <v>0</v>
-      </c>
-      <c r="V2">
-        <v>100</v>
+      <c r="U2" t="s">
+        <v>29</v>
+      </c>
+      <c r="V2" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>